<commit_message>
feat: code for adding new class to courselist
</commit_message>
<xml_diff>
--- a/113學年度1學期牙醫病理實驗課表.xlsx
+++ b/113學年度1學期牙醫病理實驗課表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1a78db8ae5a5339/桌面/code/Python/ClassCompare/ClassCompare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_EA68154F454C28AFE05B407552905E784463EB8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CDBF272-8C53-4748-87D6-39612871CAAB}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_EA68154F454C28AFE05B40755283DE7A4AEBEBD1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5925A745-36F1-4571-BF3E-9F0A9C7B387A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
     <t>醫四, 10-12節, 謝佩伶</t>
   </si>
   <si>
-    <t>Mid-Autumn Festival</t>
+    <t>Mid-Autumn Festival; 中秋節</t>
   </si>
   <si>
     <t>醫四, 10-12節, 張裕煒</t>
@@ -442,14 +442,10 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.75" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>